<commit_message>
IISIM 2.3.2, IISE 1.0.8: Inputting Medication Orders & Doses @ IISE - IISE: Added ability to enter medication orders via PanelChart   - PropertyRxOrder added as view for editing Rx Orders   - ListBox used for navigating list of currently present Rx orders   - Add/Remove buttons for adding or removing Rx orders from ListBox   - UI/UX functionality testing and debugging - IISIM: Implementing Chart   - Implemented changes to Chart based on Scenario.Step changes   - Ported population of Rx doses to IISE   - Partial implementation of ChartMAR population of Rx orders/doses
</commit_message>
<xml_diff>
--- a/II Library/Localization Strings.xlsx
+++ b/II Library/Localization Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0439D0-19A9-47EC-A400-CED95D05A137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FC2AB2-E020-4CCE-9F4C-A1F15631A945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7210" yWindow="2910" windowWidth="28800" windowHeight="15460" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5106" uniqueCount="4174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5164" uniqueCount="4232">
   <si>
     <t>Temperature</t>
   </si>
@@ -12547,6 +12547,180 @@
   </si>
   <si>
     <t>_Close</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodUnits:Hour</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodUnits:Day</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodUnits:Week</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodTypes:PRN</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodTypes:Once</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodTypes:Repeats</t>
+  </si>
+  <si>
+    <t>PRN</t>
+  </si>
+  <si>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>Repeats</t>
+  </si>
+  <si>
+    <t>ENUM:Priorities:Stat</t>
+  </si>
+  <si>
+    <t>ENUM:Priorities:Now</t>
+  </si>
+  <si>
+    <t>ENUM:Priorities:Routine</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:L</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:ML</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:G</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:MG</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:MCG</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:IU</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:Puff</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:Drop</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:ML_HR</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:MCG_HR</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:ML_KG_HR</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:MCG_KG_MIN</t>
+  </si>
+  <si>
+    <t>ENUM:Routes:PO</t>
+  </si>
+  <si>
+    <t>ENUM:Routes:IV</t>
+  </si>
+  <si>
+    <t>ENUM:TimeStatuses:Pending</t>
+  </si>
+  <si>
+    <t>ENUM:TimeStatuses:Late</t>
+  </si>
+  <si>
+    <t>ENUM:AdministrationStatuses:Administered</t>
+  </si>
+  <si>
+    <t>ENUM:AdministrationStatuses:NotAdministered</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Routine</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>Administered</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>grams</t>
+  </si>
+  <si>
+    <t>mcg</t>
+  </si>
+  <si>
+    <t>mEq</t>
+  </si>
+  <si>
+    <t>ENUM:DoseUnits:MEQ</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>puffs</t>
+  </si>
+  <si>
+    <t>drops</t>
+  </si>
+  <si>
+    <t>mL/hr</t>
+  </si>
+  <si>
+    <t>mcg/hr</t>
+  </si>
+  <si>
+    <t>mL/kg/hr</t>
+  </si>
+  <si>
+    <t>mcg/kg/min</t>
+  </si>
+  <si>
+    <t>Not Administered</t>
+  </si>
+  <si>
+    <t>ENUM:PeriodUnits:Minute</t>
+  </si>
+  <si>
+    <t>Minute</t>
   </si>
 </sst>
 </file>
@@ -12930,28 +13104,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P351"/>
+  <dimension ref="A1:P381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A245" sqref="A245"/>
+      <pane ySplit="1" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B353" sqref="B353"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="60.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="60.7265625" style="2"/>
-    <col min="3" max="4" width="60.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="60.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="60.7265625" style="3" customWidth="1"/>
-    <col min="7" max="8" width="60.7265625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="60.7265625" style="3" customWidth="1"/>
-    <col min="11" max="15" width="60.7265625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="60.7265625" style="3"/>
-    <col min="17" max="16384" width="60.7265625" style="2"/>
+    <col min="1" max="1" width="41.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" style="2"/>
+    <col min="3" max="4" width="60.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="60.7109375" style="3" customWidth="1"/>
+    <col min="11" max="15" width="60.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="60.7109375" style="3"/>
+    <col min="17" max="16384" width="60.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -13001,7 +13175,7 @@
         <v>3652</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3973</v>
       </c>
@@ -13051,7 +13225,7 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3974</v>
       </c>
@@ -13101,7 +13275,7 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -13151,7 +13325,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>84</v>
       </c>
@@ -13201,7 +13375,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>85</v>
       </c>
@@ -13251,7 +13425,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3292</v>
       </c>
@@ -13301,8 +13475,8 @@
         <v>3309</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>365</v>
       </c>
@@ -13352,7 +13526,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>332</v>
       </c>
@@ -13402,7 +13576,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>359</v>
       </c>
@@ -13452,7 +13626,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>699</v>
       </c>
@@ -13502,7 +13676,7 @@
         <v>2096</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1021</v>
       </c>
@@ -13552,7 +13726,7 @@
         <v>2097</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1203</v>
       </c>
@@ -13602,7 +13776,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>3466</v>
       </c>
@@ -13652,7 +13826,7 @@
         <v>3578</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>4168</v>
       </c>
@@ -13662,8 +13836,8 @@
       <c r="D17" s="11"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1044</v>
       </c>
@@ -13713,7 +13887,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1043</v>
       </c>
@@ -13763,8 +13937,8 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>389</v>
       </c>
@@ -13814,7 +13988,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>390</v>
       </c>
@@ -13864,7 +14038,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>391</v>
       </c>
@@ -13914,7 +14088,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>392</v>
       </c>
@@ -13964,7 +14138,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>393</v>
       </c>
@@ -14014,7 +14188,7 @@
         <v>2245</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>394</v>
       </c>
@@ -14064,7 +14238,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>395</v>
       </c>
@@ -14114,7 +14288,7 @@
         <v>2247</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>396</v>
       </c>
@@ -14164,7 +14338,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>3194</v>
       </c>
@@ -14214,7 +14388,7 @@
         <v>3202</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>397</v>
       </c>
@@ -14264,7 +14438,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>398</v>
       </c>
@@ -14314,7 +14488,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>399</v>
       </c>
@@ -14364,7 +14538,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>2848</v>
       </c>
@@ -14414,7 +14588,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>2850</v>
       </c>
@@ -14464,7 +14638,7 @@
         <v>2888</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>400</v>
       </c>
@@ -14514,7 +14688,7 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>2849</v>
       </c>
@@ -14564,7 +14738,7 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>401</v>
       </c>
@@ -14614,7 +14788,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>402</v>
       </c>
@@ -14664,7 +14838,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>403</v>
       </c>
@@ -14714,7 +14888,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>404</v>
       </c>
@@ -14764,7 +14938,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>405</v>
       </c>
@@ -14814,7 +14988,7 @@
         <v>2257</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>406</v>
       </c>
@@ -14864,7 +15038,7 @@
         <v>2258</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>407</v>
       </c>
@@ -14914,7 +15088,7 @@
         <v>2259</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>408</v>
       </c>
@@ -14964,7 +15138,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>409</v>
       </c>
@@ -15014,7 +15188,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>410</v>
       </c>
@@ -15064,7 +15238,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>411</v>
       </c>
@@ -15114,7 +15288,7 @@
         <v>2263</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>412</v>
       </c>
@@ -15164,7 +15338,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>388</v>
       </c>
@@ -15214,7 +15388,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>2786</v>
       </c>
@@ -15264,7 +15438,7 @@
         <v>2808</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>415</v>
       </c>
@@ -15314,7 +15488,7 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>2787</v>
       </c>
@@ -15364,7 +15538,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>2788</v>
       </c>
@@ -15414,7 +15588,7 @@
         <v>2809</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>2789</v>
       </c>
@@ -15464,7 +15638,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>2847</v>
       </c>
@@ -15514,7 +15688,7 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>414</v>
       </c>
@@ -15564,7 +15738,7 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>2904</v>
       </c>
@@ -15614,7 +15788,7 @@
         <v>2908</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>2920</v>
       </c>
@@ -15664,7 +15838,7 @@
         <v>2924</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>2936</v>
       </c>
@@ -15714,7 +15888,7 @@
         <v>2940</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>2952</v>
       </c>
@@ -15764,7 +15938,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>4103</v>
       </c>
@@ -15814,7 +15988,7 @@
         <v>4119</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>998</v>
       </c>
@@ -15864,7 +16038,7 @@
         <v>3631</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>999</v>
       </c>
@@ -15914,7 +16088,7 @@
         <v>3632</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>1000</v>
       </c>
@@ -15964,7 +16138,7 @@
         <v>3633</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>1001</v>
       </c>
@@ -16014,7 +16188,7 @@
         <v>3634</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>2984</v>
       </c>
@@ -16064,7 +16238,7 @@
         <v>3029</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>2985</v>
       </c>
@@ -16111,7 +16285,7 @@
         <v>3042</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>2986</v>
       </c>
@@ -16161,7 +16335,7 @@
         <v>3037</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>2987</v>
       </c>
@@ -16211,7 +16385,7 @@
         <v>3021</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>5</v>
       </c>
@@ -16261,7 +16435,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>3060</v>
       </c>
@@ -16311,7 +16485,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>6</v>
       </c>
@@ -16361,7 +16535,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>7</v>
       </c>
@@ -16411,7 +16585,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>8</v>
       </c>
@@ -16461,7 +16635,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>3662</v>
       </c>
@@ -16511,7 +16685,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>3672</v>
       </c>
@@ -16561,7 +16735,7 @@
         <v>3801</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>3664</v>
       </c>
@@ -16611,7 +16785,7 @@
         <v>3707</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>3665</v>
       </c>
@@ -16661,7 +16835,7 @@
         <v>3718</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>334</v>
       </c>
@@ -16711,7 +16885,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>3919</v>
       </c>
@@ -16761,7 +16935,7 @@
         <v>3931</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>336</v>
       </c>
@@ -16811,7 +16985,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>9</v>
       </c>
@@ -16861,7 +17035,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>3686</v>
       </c>
@@ -16911,7 +17085,7 @@
         <v>3835</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>10</v>
       </c>
@@ -16961,8 +17135,8 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>30</v>
       </c>
@@ -17012,7 +17186,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>31</v>
       </c>
@@ -17062,7 +17236,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>32</v>
       </c>
@@ -17112,7 +17286,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>33</v>
       </c>
@@ -17162,7 +17336,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="94" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>34</v>
       </c>
@@ -17212,7 +17386,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="95" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>35</v>
       </c>
@@ -17262,7 +17436,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="96" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>972</v>
       </c>
@@ -17312,7 +17486,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="97" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>36</v>
       </c>
@@ -17362,7 +17536,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>37</v>
       </c>
@@ -17412,7 +17586,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="99" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>4164</v>
       </c>
@@ -17420,7 +17594,7 @@
         <v>4166</v>
       </c>
     </row>
-    <row r="100" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
         <v>4165</v>
       </c>
@@ -17428,9 +17602,9 @@
         <v>4167</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="102" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="103" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>2438</v>
       </c>
@@ -17480,7 +17654,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>2441</v>
       </c>
@@ -17530,7 +17704,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="105" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>3290</v>
       </c>
@@ -17580,8 +17754,8 @@
         <v>3306</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="107" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>2902</v>
       </c>
@@ -17631,7 +17805,7 @@
         <v>3057</v>
       </c>
     </row>
-    <row r="108" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>3116</v>
       </c>
@@ -17681,7 +17855,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="109" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>3108</v>
       </c>
@@ -17731,7 +17905,7 @@
         <v>3145</v>
       </c>
     </row>
-    <row r="110" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>3109</v>
       </c>
@@ -17781,7 +17955,7 @@
         <v>3169</v>
       </c>
     </row>
-    <row r="111" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>3110</v>
       </c>
@@ -17831,7 +18005,7 @@
         <v>3133</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>3113</v>
       </c>
@@ -17881,7 +18055,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>3076</v>
       </c>
@@ -17931,7 +18105,7 @@
         <v>3083</v>
       </c>
     </row>
-    <row r="114" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>3077</v>
       </c>
@@ -17981,8 +18155,8 @@
         <v>3106</v>
       </c>
     </row>
-    <row r="115" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="116" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>23</v>
       </c>
@@ -18032,7 +18206,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="117" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>11</v>
       </c>
@@ -18082,7 +18256,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>12</v>
       </c>
@@ -18132,7 +18306,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>13</v>
       </c>
@@ -18182,7 +18356,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="120" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>14</v>
       </c>
@@ -18232,7 +18406,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="121" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>15</v>
       </c>
@@ -18282,7 +18456,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="122" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>16</v>
       </c>
@@ -18332,7 +18506,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="123" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>17</v>
       </c>
@@ -18382,7 +18556,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>18</v>
       </c>
@@ -18432,7 +18606,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="125" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>3471</v>
       </c>
@@ -18482,7 +18656,7 @@
         <v>3485</v>
       </c>
     </row>
-    <row r="126" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>19</v>
       </c>
@@ -18532,7 +18706,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="127" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>2345</v>
       </c>
@@ -18582,7 +18756,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="128" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>2363</v>
       </c>
@@ -18632,7 +18806,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="129" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>20</v>
       </c>
@@ -18682,7 +18856,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="130" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>21</v>
       </c>
@@ -18732,7 +18906,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>2717</v>
       </c>
@@ -18782,7 +18956,7 @@
         <v>2728</v>
       </c>
     </row>
-    <row r="132" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>22</v>
       </c>
@@ -18832,7 +19006,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>24</v>
       </c>
@@ -18882,7 +19056,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="134" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>25</v>
       </c>
@@ -18932,7 +19106,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="135" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>26</v>
       </c>
@@ -18982,7 +19156,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="136" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>27</v>
       </c>
@@ -19032,7 +19206,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="137" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>2413</v>
       </c>
@@ -19082,7 +19256,7 @@
         <v>2425</v>
       </c>
     </row>
-    <row r="138" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>2721</v>
       </c>
@@ -19132,7 +19306,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="139" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>2722</v>
       </c>
@@ -19182,7 +19356,7 @@
         <v>2755</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>2967</v>
       </c>
@@ -19232,7 +19406,7 @@
         <v>2971</v>
       </c>
     </row>
-    <row r="141" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>4035</v>
       </c>
@@ -19282,7 +19456,7 @@
         <v>4046</v>
       </c>
     </row>
-    <row r="142" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>4039</v>
       </c>
@@ -19332,7 +19506,7 @@
         <v>4080</v>
       </c>
     </row>
-    <row r="143" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>4036</v>
       </c>
@@ -19382,7 +19556,7 @@
         <v>4079</v>
       </c>
     </row>
-    <row r="144" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>2623</v>
       </c>
@@ -19432,7 +19606,7 @@
         <v>2638</v>
       </c>
     </row>
-    <row r="145" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>28</v>
       </c>
@@ -19482,7 +19656,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="146" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>29</v>
       </c>
@@ -19532,7 +19706,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="147" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>985</v>
       </c>
@@ -19582,7 +19756,7 @@
         <v>3488</v>
       </c>
     </row>
-    <row r="148" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>981</v>
       </c>
@@ -19632,7 +19806,7 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="149" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>4120</v>
       </c>
@@ -19682,7 +19856,7 @@
         <v>4124</v>
       </c>
     </row>
-    <row r="150" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>982</v>
       </c>
@@ -19732,7 +19906,7 @@
         <v>3509</v>
       </c>
     </row>
-    <row r="151" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>983</v>
       </c>
@@ -19782,7 +19956,7 @@
         <v>3869</v>
       </c>
     </row>
-    <row r="152" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>989</v>
       </c>
@@ -19832,7 +20006,7 @@
         <v>3562</v>
       </c>
     </row>
-    <row r="153" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>984</v>
       </c>
@@ -19882,7 +20056,7 @@
         <v>3563</v>
       </c>
     </row>
-    <row r="154" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>4121</v>
       </c>
@@ -19932,8 +20106,8 @@
         <v>4156</v>
       </c>
     </row>
-    <row r="155" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="156" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>2611</v>
       </c>
@@ -19983,7 +20157,7 @@
         <v>2639</v>
       </c>
     </row>
-    <row r="157" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>2612</v>
       </c>
@@ -20033,7 +20207,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="158" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>2613</v>
       </c>
@@ -20083,7 +20257,7 @@
         <v>2641</v>
       </c>
     </row>
-    <row r="159" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>2614</v>
       </c>
@@ -20133,7 +20307,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="160" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>2615</v>
       </c>
@@ -20183,7 +20357,7 @@
         <v>2643</v>
       </c>
     </row>
-    <row r="161" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>2616</v>
       </c>
@@ -20233,7 +20407,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="163" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>1247</v>
       </c>
@@ -20283,7 +20457,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="164" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>1218</v>
       </c>
@@ -20333,7 +20507,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="165" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>1219</v>
       </c>
@@ -20383,7 +20557,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="166" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>1216</v>
       </c>
@@ -20433,7 +20607,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="167" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>1205</v>
       </c>
@@ -20483,7 +20657,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="168" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>1206</v>
       </c>
@@ -20533,7 +20707,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="169" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>1213</v>
       </c>
@@ -20583,7 +20757,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="170" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>1207</v>
       </c>
@@ -20633,7 +20807,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="171" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>1208</v>
       </c>
@@ -20683,7 +20857,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="172" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>1220</v>
       </c>
@@ -20733,7 +20907,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="173" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>1221</v>
       </c>
@@ -20783,7 +20957,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="174" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>1222</v>
       </c>
@@ -20833,7 +21007,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="175" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>1227</v>
       </c>
@@ -20883,7 +21057,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="176" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>1228</v>
       </c>
@@ -20933,7 +21107,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="177" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>2381</v>
       </c>
@@ -20983,7 +21157,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="178" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>2767</v>
       </c>
@@ -21033,7 +21207,7 @@
         <v>2774</v>
       </c>
     </row>
-    <row r="179" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>1232</v>
       </c>
@@ -21083,7 +21257,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="180" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>1245</v>
       </c>
@@ -21133,7 +21307,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="181" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>1246</v>
       </c>
@@ -21174,7 +21348,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="182" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>1237</v>
       </c>
@@ -21224,7 +21398,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="183" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>1238</v>
       </c>
@@ -21274,7 +21448,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="184" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>1235</v>
       </c>
@@ -21324,7 +21498,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="185" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>1236</v>
       </c>
@@ -21374,7 +21548,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="186" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>1243</v>
       </c>
@@ -21424,8 +21598,8 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="187" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="188" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>1195</v>
       </c>
@@ -21475,7 +21649,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="189" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>1041</v>
       </c>
@@ -21525,7 +21699,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="190" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>1047</v>
       </c>
@@ -21575,7 +21749,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="191" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>1196</v>
       </c>
@@ -21625,7 +21799,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="192" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>1197</v>
       </c>
@@ -21675,7 +21849,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="193" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>1202</v>
       </c>
@@ -21725,7 +21899,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="194" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>1049</v>
       </c>
@@ -21775,7 +21949,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="195" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>1050</v>
       </c>
@@ -21825,7 +21999,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="196" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>1054</v>
       </c>
@@ -21875,7 +22049,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="197" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>2784</v>
       </c>
@@ -21925,7 +22099,7 @@
         <v>2774</v>
       </c>
     </row>
-    <row r="198" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>1186</v>
       </c>
@@ -21975,7 +22149,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="199" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>1023</v>
       </c>
@@ -22025,7 +22199,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="200" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>1024</v>
       </c>
@@ -22075,7 +22249,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="201" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>1027</v>
       </c>
@@ -22125,7 +22299,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="202" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>1028</v>
       </c>
@@ -22175,7 +22349,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="203" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>1032</v>
       </c>
@@ -22225,7 +22399,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="204" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>1033</v>
       </c>
@@ -22275,7 +22449,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="205" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>1034</v>
       </c>
@@ -22325,7 +22499,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="206" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>1192</v>
       </c>
@@ -22372,7 +22546,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="207" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>1191</v>
       </c>
@@ -22419,7 +22593,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="208" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>1056</v>
       </c>
@@ -22469,7 +22643,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="209" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>1189</v>
       </c>
@@ -22516,7 +22690,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="210" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>1190</v>
       </c>
@@ -22563,8 +22737,8 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="211" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="212" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="10" t="s">
         <v>4170</v>
       </c>
@@ -22572,7 +22746,7 @@
         <v>4171</v>
       </c>
     </row>
-    <row r="213" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>1007</v>
       </c>
@@ -22622,7 +22796,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="214" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>1008</v>
       </c>
@@ -22672,7 +22846,7 @@
         <v>2191</v>
       </c>
     </row>
-    <row r="215" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>1009</v>
       </c>
@@ -22722,7 +22896,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="216" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>1018</v>
       </c>
@@ -22772,7 +22946,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="217" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>1010</v>
       </c>
@@ -22822,7 +22996,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="218" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>1019</v>
       </c>
@@ -22872,7 +23046,7 @@
         <v>2201</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>2343</v>
       </c>
@@ -22922,7 +23096,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="220" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>2344</v>
       </c>
@@ -22972,7 +23146,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="221" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>1011</v>
       </c>
@@ -23022,7 +23196,7 @@
         <v>2194</v>
       </c>
     </row>
-    <row r="222" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>1013</v>
       </c>
@@ -23072,7 +23246,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="223" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>1012</v>
       </c>
@@ -23122,7 +23296,7 @@
         <v>2195</v>
       </c>
     </row>
-    <row r="224" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>4081</v>
       </c>
@@ -23172,7 +23346,7 @@
         <v>4089</v>
       </c>
     </row>
-    <row r="225" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>4083</v>
       </c>
@@ -23222,7 +23396,7 @@
         <v>4085</v>
       </c>
     </row>
-    <row r="226" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>4084</v>
       </c>
@@ -23272,7 +23446,7 @@
         <v>4086</v>
       </c>
     </row>
-    <row r="227" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>4087</v>
       </c>
@@ -23322,7 +23496,7 @@
         <v>4088</v>
       </c>
     </row>
-    <row r="228" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>3875</v>
       </c>
@@ -23372,7 +23546,7 @@
         <v>3918</v>
       </c>
     </row>
-    <row r="229" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>3876</v>
       </c>
@@ -23422,7 +23596,7 @@
         <v>3917</v>
       </c>
     </row>
-    <row r="230" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>3877</v>
       </c>
@@ -23472,7 +23646,7 @@
         <v>3916</v>
       </c>
     </row>
-    <row r="231" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>3935</v>
       </c>
@@ -23522,7 +23696,7 @@
         <v>3943</v>
       </c>
     </row>
-    <row r="232" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>3936</v>
       </c>
@@ -23572,7 +23746,7 @@
         <v>3944</v>
       </c>
     </row>
-    <row r="233" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>3937</v>
       </c>
@@ -23622,7 +23796,7 @@
         <v>3945</v>
       </c>
     </row>
-    <row r="234" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>4157</v>
       </c>
@@ -23672,7 +23846,7 @@
         <v>3931</v>
       </c>
     </row>
-    <row r="235" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>4163</v>
       </c>
@@ -23722,7 +23896,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="236" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>4159</v>
       </c>
@@ -23772,7 +23946,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="237" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>4160</v>
       </c>
@@ -23822,7 +23996,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="238" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>1014</v>
       </c>
@@ -23872,7 +24046,7 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="239" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>3243</v>
       </c>
@@ -23922,7 +24096,7 @@
         <v>3263</v>
       </c>
     </row>
-    <row r="240" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>3242</v>
       </c>
@@ -23972,7 +24146,7 @@
         <v>3258</v>
       </c>
     </row>
-    <row r="241" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>3274</v>
       </c>
@@ -24022,7 +24196,7 @@
         <v>3279</v>
       </c>
     </row>
-    <row r="242" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>1015</v>
       </c>
@@ -24072,7 +24246,7 @@
         <v>2198</v>
       </c>
     </row>
-    <row r="243" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>3322</v>
       </c>
@@ -24122,7 +24296,7 @@
         <v>3337</v>
       </c>
     </row>
-    <row r="244" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3" t="s">
         <v>3323</v>
       </c>
@@ -24172,7 +24346,7 @@
         <v>3343</v>
       </c>
     </row>
-    <row r="245" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="10" t="s">
         <v>4172</v>
       </c>
@@ -24180,7 +24354,7 @@
         <v>4173</v>
       </c>
     </row>
-    <row r="246" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
         <v>1016</v>
       </c>
@@ -24230,7 +24404,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="247" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
         <v>1017</v>
       </c>
@@ -24280,7 +24454,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="248" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
         <v>1020</v>
       </c>
@@ -24330,7 +24504,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="249" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>1039</v>
       </c>
@@ -24380,7 +24554,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="250" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
         <v>3212</v>
       </c>
@@ -24430,7 +24604,7 @@
         <v>3239</v>
       </c>
     </row>
-    <row r="252" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
         <v>441</v>
       </c>
@@ -24480,7 +24654,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="253" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
         <v>442</v>
       </c>
@@ -24530,7 +24704,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="254" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
         <v>443</v>
       </c>
@@ -24580,7 +24754,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="255" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>444</v>
       </c>
@@ -24630,7 +24804,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="256" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
         <v>445</v>
       </c>
@@ -24680,7 +24854,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="257" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>446</v>
       </c>
@@ -24730,7 +24904,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="258" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>447</v>
       </c>
@@ -24780,7 +24954,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="259" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>448</v>
       </c>
@@ -24830,7 +25004,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="260" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>3473</v>
       </c>
@@ -24880,7 +25054,7 @@
         <v>3485</v>
       </c>
     </row>
-    <row r="261" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>698</v>
       </c>
@@ -24930,7 +25104,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="262" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>2346</v>
       </c>
@@ -24980,7 +25154,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="263" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>2366</v>
       </c>
@@ -25030,7 +25204,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="264" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>1200</v>
       </c>
@@ -25080,7 +25254,7 @@
         <v>2219</v>
       </c>
     </row>
-    <row r="265" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>1226</v>
       </c>
@@ -25130,7 +25304,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="266" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
         <v>1040</v>
       </c>
@@ -25180,8 +25354,8 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="267" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="268" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
         <v>694</v>
       </c>
@@ -25231,7 +25405,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="269" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>3210</v>
       </c>
@@ -25281,7 +25455,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="270" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>3211</v>
       </c>
@@ -25331,10 +25505,10 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="271" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J271" s="4"/>
     </row>
-    <row r="272" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
         <v>461</v>
       </c>
@@ -25384,7 +25558,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="273" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>462</v>
       </c>
@@ -25434,7 +25608,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="274" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>463</v>
       </c>
@@ -25484,7 +25658,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="275" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>478</v>
       </c>
@@ -25534,7 +25708,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="276" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>2347</v>
       </c>
@@ -25584,7 +25758,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="277" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>2365</v>
       </c>
@@ -25634,7 +25808,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="278" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>1030</v>
       </c>
@@ -25684,7 +25858,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="279" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>464</v>
       </c>
@@ -25734,7 +25908,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="280" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>465</v>
       </c>
@@ -25784,7 +25958,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="281" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>466</v>
       </c>
@@ -25834,7 +26008,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="282" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
         <v>467</v>
       </c>
@@ -25884,7 +26058,7 @@
         <v>2296</v>
       </c>
     </row>
-    <row r="283" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
         <v>468</v>
       </c>
@@ -25934,7 +26108,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="284" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
         <v>469</v>
       </c>
@@ -25984,7 +26158,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="285" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>470</v>
       </c>
@@ -26034,7 +26208,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="286" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
         <v>471</v>
       </c>
@@ -26084,7 +26258,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="287" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
         <v>472</v>
       </c>
@@ -26134,7 +26308,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="288" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="s">
         <v>473</v>
       </c>
@@ -26184,7 +26358,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="289" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
         <v>474</v>
       </c>
@@ -26234,7 +26408,7 @@
         <v>2303</v>
       </c>
     </row>
-    <row r="290" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
         <v>475</v>
       </c>
@@ -26284,7 +26458,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="291" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
         <v>476</v>
       </c>
@@ -26334,7 +26508,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="292" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
         <v>477</v>
       </c>
@@ -26384,7 +26558,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="293" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
         <v>704</v>
       </c>
@@ -26434,7 +26608,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="294" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
         <v>705</v>
       </c>
@@ -26484,7 +26658,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="295" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>706</v>
       </c>
@@ -26534,7 +26708,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="296" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="s">
         <v>707</v>
       </c>
@@ -26584,7 +26758,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="297" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
         <v>708</v>
       </c>
@@ -26634,7 +26808,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="298" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
         <v>709</v>
       </c>
@@ -26684,7 +26858,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="299" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
         <v>710</v>
       </c>
@@ -26734,7 +26908,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="300" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
         <v>711</v>
       </c>
@@ -26784,7 +26958,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="301" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
         <v>712</v>
       </c>
@@ -26834,7 +27008,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="302" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
         <v>713</v>
       </c>
@@ -26884,7 +27058,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="303" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>714</v>
       </c>
@@ -26934,7 +27108,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="304" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
         <v>715</v>
       </c>
@@ -26984,7 +27158,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="305" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>3468</v>
       </c>
@@ -27034,7 +27208,7 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="306" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
         <v>3469</v>
       </c>
@@ -27084,8 +27258,8 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="307" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="308" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="308" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>990</v>
       </c>
@@ -27135,7 +27309,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="309" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>991</v>
       </c>
@@ -27185,7 +27359,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="310" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
         <v>992</v>
       </c>
@@ -27235,7 +27409,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="311" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>993</v>
       </c>
@@ -27285,8 +27459,8 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="312" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="313" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="313" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>2412</v>
       </c>
@@ -27336,8 +27510,8 @@
         <v>3857</v>
       </c>
     </row>
-    <row r="314" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="315" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="315" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="s">
         <v>4003</v>
       </c>
@@ -27387,7 +27561,7 @@
         <v>4007</v>
       </c>
     </row>
-    <row r="316" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
         <v>4004</v>
       </c>
@@ -27437,8 +27611,8 @@
         <v>4025</v>
       </c>
     </row>
-    <row r="317" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="318" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="318" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="s">
         <v>40</v>
       </c>
@@ -27488,7 +27662,7 @@
         <v>2233</v>
       </c>
     </row>
-    <row r="319" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3" t="s">
         <v>38</v>
       </c>
@@ -27538,7 +27712,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="320" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3" t="s">
         <v>39</v>
       </c>
@@ -27588,8 +27762,8 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="321" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="322" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="322" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3" t="s">
         <v>3656</v>
       </c>
@@ -27639,7 +27813,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="323" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
         <v>3657</v>
       </c>
@@ -27689,8 +27863,8 @@
         <v>2239</v>
       </c>
     </row>
-    <row r="324" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="325" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="325" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A325" s="3" t="s">
         <v>3660</v>
       </c>
@@ -27740,7 +27914,7 @@
         <v>3704</v>
       </c>
     </row>
-    <row r="326" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A326" s="3" t="s">
         <v>3661</v>
       </c>
@@ -27790,10 +27964,10 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="327" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G327" s="4"/>
     </row>
-    <row r="328" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A328" s="3" t="s">
         <v>3670</v>
       </c>
@@ -27843,7 +28017,7 @@
         <v>3707</v>
       </c>
     </row>
-    <row r="329" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A329" s="3" t="s">
         <v>3671</v>
       </c>
@@ -27893,7 +28067,7 @@
         <v>3718</v>
       </c>
     </row>
-    <row r="330" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A330" s="3" t="s">
         <v>3688</v>
       </c>
@@ -27943,7 +28117,7 @@
         <v>3721</v>
       </c>
     </row>
-    <row r="331" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A331" s="3" t="s">
         <v>3690</v>
       </c>
@@ -27993,7 +28167,7 @@
         <v>3732</v>
       </c>
     </row>
-    <row r="332" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="s">
         <v>3676</v>
       </c>
@@ -28043,7 +28217,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="333" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A333" s="3" t="s">
         <v>3677</v>
       </c>
@@ -28093,7 +28267,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="334" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A334" s="3" t="s">
         <v>3678</v>
       </c>
@@ -28143,7 +28317,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="335" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A335" s="3" t="s">
         <v>3674</v>
       </c>
@@ -28193,7 +28367,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="336" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A336" s="3" t="s">
         <v>3675</v>
       </c>
@@ -28243,7 +28417,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="337" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
         <v>3679</v>
       </c>
@@ -28293,7 +28467,7 @@
         <v>2603</v>
       </c>
     </row>
-    <row r="338" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A338" s="3" t="s">
         <v>3680</v>
       </c>
@@ -28343,7 +28517,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="339" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A339" s="3" t="s">
         <v>3681</v>
       </c>
@@ -28393,7 +28567,7 @@
         <v>2605</v>
       </c>
     </row>
-    <row r="340" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A340" s="3" t="s">
         <v>3682</v>
       </c>
@@ -28443,7 +28617,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="341" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
         <v>3683</v>
       </c>
@@ -28493,7 +28667,7 @@
         <v>2607</v>
       </c>
     </row>
-    <row r="342" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A342" s="3" t="s">
         <v>3684</v>
       </c>
@@ -28543,7 +28717,7 @@
         <v>2609</v>
       </c>
     </row>
-    <row r="344" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="s">
         <v>3364</v>
       </c>
@@ -28593,7 +28767,7 @@
         <v>3372</v>
       </c>
     </row>
-    <row r="345" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
         <v>3687</v>
       </c>
@@ -28643,7 +28817,7 @@
         <v>3763</v>
       </c>
     </row>
-    <row r="346" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
         <v>3354</v>
       </c>
@@ -28693,7 +28867,7 @@
         <v>3395</v>
       </c>
     </row>
-    <row r="347" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3" t="s">
         <v>3356</v>
       </c>
@@ -28743,7 +28917,7 @@
         <v>3396</v>
       </c>
     </row>
-    <row r="348" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3" t="s">
         <v>3357</v>
       </c>
@@ -28793,7 +28967,7 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="349" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3" t="s">
         <v>3358</v>
       </c>
@@ -28843,7 +29017,7 @@
         <v>3431</v>
       </c>
     </row>
-    <row r="350" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
         <v>3359</v>
       </c>
@@ -28893,7 +29067,7 @@
         <v>3447</v>
       </c>
     </row>
-    <row r="351" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
         <v>3366</v>
       </c>
@@ -28941,6 +29115,238 @@
       </c>
       <c r="P351" s="3" t="s">
         <v>3463</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="10" t="s">
+        <v>4230</v>
+      </c>
+      <c r="B353" s="10" t="s">
+        <v>4231</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="10" t="s">
+        <v>4174</v>
+      </c>
+      <c r="B354" s="10" t="s">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="10" t="s">
+        <v>4175</v>
+      </c>
+      <c r="B355" s="10" t="s">
+        <v>4178</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="10" t="s">
+        <v>4176</v>
+      </c>
+      <c r="B356" s="10" t="s">
+        <v>4179</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="10" t="s">
+        <v>4180</v>
+      </c>
+      <c r="B357" s="10" t="s">
+        <v>4183</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="10" t="s">
+        <v>4181</v>
+      </c>
+      <c r="B358" s="10" t="s">
+        <v>4184</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A359" s="10" t="s">
+        <v>4182</v>
+      </c>
+      <c r="B359" s="10" t="s">
+        <v>4185</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="10" t="s">
+        <v>4186</v>
+      </c>
+      <c r="B360" s="10" t="s">
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="10" t="s">
+        <v>4187</v>
+      </c>
+      <c r="B361" s="10" t="s">
+        <v>4208</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="10" t="s">
+        <v>4188</v>
+      </c>
+      <c r="B362" s="10" t="s">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="10" t="s">
+        <v>4189</v>
+      </c>
+      <c r="B363" s="10" t="s">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="10" t="s">
+        <v>4190</v>
+      </c>
+      <c r="B364" s="10" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="10" t="s">
+        <v>4191</v>
+      </c>
+      <c r="B365" s="10" t="s">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="10" t="s">
+        <v>4192</v>
+      </c>
+      <c r="B366" s="10" t="s">
+        <v>4217</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="10" t="s">
+        <v>4193</v>
+      </c>
+      <c r="B367" s="10" t="s">
+        <v>4219</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="10" t="s">
+        <v>4221</v>
+      </c>
+      <c r="B368" s="10" t="s">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A369" s="10" t="s">
+        <v>4194</v>
+      </c>
+      <c r="B369" s="10" t="s">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A370" s="10" t="s">
+        <v>4195</v>
+      </c>
+      <c r="B370" s="10" t="s">
+        <v>4223</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A371" s="10" t="s">
+        <v>4196</v>
+      </c>
+      <c r="B371" s="10" t="s">
+        <v>4224</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="10" t="s">
+        <v>4197</v>
+      </c>
+      <c r="B372" s="10" t="s">
+        <v>4225</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A373" s="10" t="s">
+        <v>4198</v>
+      </c>
+      <c r="B373" s="10" t="s">
+        <v>4226</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A374" s="10" t="s">
+        <v>4199</v>
+      </c>
+      <c r="B374" s="10" t="s">
+        <v>4227</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A375" s="10" t="s">
+        <v>4200</v>
+      </c>
+      <c r="B375" s="10" t="s">
+        <v>4228</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="10" t="s">
+        <v>4201</v>
+      </c>
+      <c r="B376" s="10" t="s">
+        <v>4211</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="10" t="s">
+        <v>4202</v>
+      </c>
+      <c r="B377" s="10" t="s">
+        <v>4212</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="10" t="s">
+        <v>4203</v>
+      </c>
+      <c r="B378" s="10" t="s">
+        <v>4213</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A379" s="10" t="s">
+        <v>4204</v>
+      </c>
+      <c r="B379" s="10" t="s">
+        <v>4214</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="10" t="s">
+        <v>4205</v>
+      </c>
+      <c r="B380" s="10" t="s">
+        <v>4215</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="10" t="s">
+        <v>4206</v>
+      </c>
+      <c r="B381" s="10" t="s">
+        <v>4229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IISIM 2.5.9-1: Strings localized for supported languages
</commit_message>
<xml_diff>
--- a/II Library/Localization Strings.xlsx
+++ b/II Library/Localization Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\infirmary-integrated\II Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0964C144-1C5B-43EE-BB5D-9A4E3F2AF402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FBBE68-BEDA-4248-B764-E0B1B6538764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15410" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6110" uniqueCount="5089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6152" uniqueCount="5131">
   <si>
     <t>Temperature</t>
   </si>
@@ -15292,6 +15292,132 @@
   </si>
   <si>
     <t>MENU:MenuColorSchemeGrid</t>
+  </si>
+  <si>
+    <t>تمكين الصوت</t>
+  </si>
+  <si>
+    <t>تعطيل الصوت</t>
+  </si>
+  <si>
+    <t>ድምጽ አሰናክል</t>
+  </si>
+  <si>
+    <t>ድምጽን አንቃ</t>
+  </si>
+  <si>
+    <t>Audio aktivieren</t>
+  </si>
+  <si>
+    <t>Deaktiviere Audio</t>
+  </si>
+  <si>
+    <t>Desactivar el audio</t>
+  </si>
+  <si>
+    <t>Activar audio</t>
+  </si>
+  <si>
+    <t>Activer le son</t>
+  </si>
+  <si>
+    <t>Désactiver le son</t>
+  </si>
+  <si>
+    <t>Disattiva l'audio</t>
+  </si>
+  <si>
+    <t>Attiva l'audio</t>
+  </si>
+  <si>
+    <t>Ativar áudio</t>
+  </si>
+  <si>
+    <t>Desativar áudio</t>
+  </si>
+  <si>
+    <t>Деактивировать звук</t>
+  </si>
+  <si>
+    <t>Включить звук</t>
+  </si>
+  <si>
+    <t>Washa sauti</t>
+  </si>
+  <si>
+    <t>Zima sauti</t>
+  </si>
+  <si>
+    <t>停用音频</t>
+  </si>
+  <si>
+    <t>激活音频</t>
+  </si>
+  <si>
+    <t>오디오 활성화</t>
+  </si>
+  <si>
+    <t>오디오 비활성화</t>
+  </si>
+  <si>
+    <t>ऑडियो निष्क्रिय करें</t>
+  </si>
+  <si>
+    <t>ऑडियो सक्रिय करें</t>
+  </si>
+  <si>
+    <t>הפעל אודיו</t>
+  </si>
+  <si>
+    <t>השבת את האודיו</t>
+  </si>
+  <si>
+    <t>صدا را غیرفعال کنید</t>
+  </si>
+  <si>
+    <t>صدا را فعال کنید</t>
+  </si>
+  <si>
+    <t>الگوی مربع</t>
+  </si>
+  <si>
+    <t>نمط الشبكة المربعة</t>
+  </si>
+  <si>
+    <t>የካሬ ፍርግርግ ንድፍ</t>
+  </si>
+  <si>
+    <t>Quadratisches Gitterdesign</t>
+  </si>
+  <si>
+    <t>Grille</t>
+  </si>
+  <si>
+    <t>Cuadrícula</t>
+  </si>
+  <si>
+    <t>רשת מרובעת</t>
+  </si>
+  <si>
+    <t>वर्गाकार ग्रिड पैटर्न</t>
+  </si>
+  <si>
+    <t>Motivo quadrato</t>
+  </si>
+  <si>
+    <t>Padrão quadrado</t>
+  </si>
+  <si>
+    <t>정사각형 패턴</t>
+  </si>
+  <si>
+    <t>Квадратная сетка</t>
+  </si>
+  <si>
+    <t>Gridi ya mraba</t>
+  </si>
+  <si>
+    <t>方形网格图案</t>
   </si>
 </sst>
 </file>
@@ -15321,18 +15447,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -15362,7 +15482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -15387,9 +15507,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -15674,9 +15791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P414"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B248" sqref="B248"/>
+      <selection pane="bottomLeft" activeCell="L236" sqref="L236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27030,48 +27147,104 @@
       </c>
     </row>
     <row r="243" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A243" s="10" t="s">
+      <c r="A243" s="3" t="s">
         <v>5083</v>
       </c>
-      <c r="B243" s="10" t="s">
+      <c r="B243" s="3" t="s">
         <v>5085</v>
       </c>
-      <c r="C243" s="10"/>
-      <c r="D243" s="10"/>
-      <c r="E243" s="10"/>
-      <c r="F243" s="10"/>
-      <c r="G243" s="10"/>
-      <c r="H243" s="10"/>
-      <c r="I243" s="10"/>
-      <c r="J243" s="10"/>
-      <c r="K243" s="10"/>
-      <c r="L243" s="10"/>
-      <c r="M243" s="10"/>
-      <c r="N243" s="10"/>
-      <c r="O243" s="10"/>
-      <c r="P243" s="10"/>
+      <c r="C243" s="3" t="s">
+        <v>5092</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>5089</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>5093</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>5116</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>5096</v>
+      </c>
+      <c r="H243" s="3" t="s">
+        <v>5097</v>
+      </c>
+      <c r="I243" s="3" t="s">
+        <v>5113</v>
+      </c>
+      <c r="J243" s="3" t="s">
+        <v>5112</v>
+      </c>
+      <c r="K243" s="3" t="s">
+        <v>5100</v>
+      </c>
+      <c r="L243" s="3" t="s">
+        <v>5109</v>
+      </c>
+      <c r="M243" s="3" t="s">
+        <v>5101</v>
+      </c>
+      <c r="N243" s="3" t="s">
+        <v>5104</v>
+      </c>
+      <c r="O243" s="3" t="s">
+        <v>5105</v>
+      </c>
+      <c r="P243" s="3" t="s">
+        <v>5108</v>
+      </c>
     </row>
     <row r="244" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A244" s="10" t="s">
+      <c r="A244" s="3" t="s">
         <v>5084</v>
       </c>
-      <c r="B244" s="10" t="s">
+      <c r="B244" s="3" t="s">
         <v>5086</v>
       </c>
-      <c r="C244" s="10"/>
-      <c r="D244" s="10"/>
-      <c r="E244" s="10"/>
-      <c r="F244" s="10"/>
-      <c r="G244" s="10"/>
-      <c r="H244" s="10"/>
-      <c r="I244" s="10"/>
-      <c r="J244" s="10"/>
-      <c r="K244" s="10"/>
-      <c r="L244" s="10"/>
-      <c r="M244" s="10"/>
-      <c r="N244" s="10"/>
-      <c r="O244" s="10"/>
-      <c r="P244" s="10"/>
+      <c r="C244" s="3" t="s">
+        <v>5091</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>5090</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>5094</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>5115</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>5095</v>
+      </c>
+      <c r="H244" s="3" t="s">
+        <v>5098</v>
+      </c>
+      <c r="I244" s="3" t="s">
+        <v>5114</v>
+      </c>
+      <c r="J244" s="3" t="s">
+        <v>5111</v>
+      </c>
+      <c r="K244" s="3" t="s">
+        <v>5099</v>
+      </c>
+      <c r="L244" s="3" t="s">
+        <v>5110</v>
+      </c>
+      <c r="M244" s="3" t="s">
+        <v>5102</v>
+      </c>
+      <c r="N244" s="3" t="s">
+        <v>5103</v>
+      </c>
+      <c r="O244" s="3" t="s">
+        <v>5106</v>
+      </c>
+      <c r="P244" s="3" t="s">
+        <v>5107</v>
+      </c>
     </row>
     <row r="245" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A245" s="3" t="s">
@@ -27374,26 +27547,54 @@
       </c>
     </row>
     <row r="251" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A251" s="10" t="s">
+      <c r="A251" s="3" t="s">
         <v>5088</v>
       </c>
-      <c r="B251" s="10" t="s">
+      <c r="B251" s="3" t="s">
         <v>5087</v>
       </c>
-      <c r="C251" s="10"/>
-      <c r="D251" s="10"/>
-      <c r="E251" s="10"/>
-      <c r="F251" s="10"/>
-      <c r="G251" s="10"/>
-      <c r="H251" s="10"/>
-      <c r="I251" s="10"/>
-      <c r="J251" s="10"/>
-      <c r="K251" s="10"/>
-      <c r="L251" s="10"/>
-      <c r="M251" s="10"/>
-      <c r="N251" s="10"/>
-      <c r="O251" s="10"/>
-      <c r="P251" s="10"/>
+      <c r="C251" s="3" t="s">
+        <v>5119</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>5118</v>
+      </c>
+      <c r="E251" s="3" t="s">
+        <v>5120</v>
+      </c>
+      <c r="F251" s="3" t="s">
+        <v>5117</v>
+      </c>
+      <c r="G251" s="3" t="s">
+        <v>5122</v>
+      </c>
+      <c r="H251" s="3" t="s">
+        <v>5121</v>
+      </c>
+      <c r="I251" s="3" t="s">
+        <v>5123</v>
+      </c>
+      <c r="J251" s="3" t="s">
+        <v>5124</v>
+      </c>
+      <c r="K251" s="3" t="s">
+        <v>5125</v>
+      </c>
+      <c r="L251" s="3" t="s">
+        <v>5127</v>
+      </c>
+      <c r="M251" s="3" t="s">
+        <v>5126</v>
+      </c>
+      <c r="N251" s="3" t="s">
+        <v>5128</v>
+      </c>
+      <c r="O251" s="3" t="s">
+        <v>5129</v>
+      </c>
+      <c r="P251" s="3" t="s">
+        <v>5130</v>
+      </c>
     </row>
     <row r="252" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A252" s="3" t="s">

</xml_diff>

<commit_message>
IISIM 2.7.12: Saving Transducers_Zeroed, Mirror Server Specification - Implemented Transducers_Zeroed into Save()/Load()   - For cardiac monitor, defibrillator, and IABP - Removed user-specific data from Mirror server calls   - Was implemented historically, never utilized; unnecessary   - Also removed from II Server/mirror_post.php - Implemented ability to specify mirror server for custom mirrors   - infirmary-integrated.com still default and TextBox.Watermark   - Implemented into Receive & Broadcast dialogs, and II.Server.Mirror.cs   - Also updated message boxes to use DialogMessage - Localization strings updated for clarity
</commit_message>
<xml_diff>
--- a/II Library/Localization Strings.xlsx
+++ b/II Library/Localization Strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5183" uniqueCount="5183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5185" uniqueCount="5185">
   <si>
     <t>Key</t>
   </si>
@@ -14628,97 +14628,97 @@
     <t>MIRROR:EnterSettings</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter settings, only using numbers and letters:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ቁጥሮችን እና ፊደሎችን ብቻ በመጠቀም ቅንብሮችን ያስገቡ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">أدخل الإعدادات ، باستخدام الأرقام والحروف فقط:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geben Sie die Einstellungen ein, verwenden Sie nur Zahlen und Buchstaben:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تنظیمات را فقط با استفاده از اعداد و حروف وارد کنید:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingrese la configuración, solo use números y letras:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrez les paramètres, utilisez uniquement des chiffres et des lettres :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">הזן הגדרות, באמצעות מספרים ואותיות בלבד:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">केवल संख्याओं और अक्षरों का उपयोग करके सेटिंग दर्ज करें:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inserisci le impostazioni, usa solo numeri e lettere:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">숫자와 문자만 사용하여 설정을 입력합니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insira as configurações, use apenas números e letras:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вводите настройки, используя только цифры и буквы.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingiza mipangilio ukitumia nambari na herufi tu.</t>
-  </si>
-  <si>
-    <t>进入设置，只使用数字和字母：</t>
+    <t xml:space="preserve">Enter settings:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ቅንብሮችን ያስገቡ፡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">أدخل الإعدادات:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einstellungen eingeben:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تنظیمات را وارد کنید:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingrese la configuración:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrez les paramètres:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">הזן הגדרות:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">सेटिंग्स दर्ज करें:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserisci le impostazioni:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">설정으로 이동:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insira as configurações:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перейдите в настройки:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingiza mipangilio:</t>
+  </si>
+  <si>
+    <t>进入设置：</t>
   </si>
   <si>
     <t>MIRROR:SettingsInvalid</t>
   </si>
   <si>
-    <t xml:space="preserve">Settings can only include letters and numbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ቅንጅቶች ፊደሎችን እና ቁጥሮችን ብቻ ሊያካትቱ ይችላሉ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">يمكن أن تتضمن الإعدادات أحرفًا وأرقامًا فقط</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Einstellungen können nur Buchstaben und Zahlen enthalten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تنظیمات فقط می توانند شامل حروف و اعداد باشند</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La configuración solo puede contener letras y números</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les paramètres ne peuvent contenir que des lettres et des chiffres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ההגדרות יכולות לכלול רק אותיות ומספרים</t>
-  </si>
-  <si>
-    <t xml:space="preserve">सेटिंग्स में केवल अक्षर और संख्याएं शामिल हो सकती हैं</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le impostazioni possono contenere solo lettere e numeri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">설정에는 문자와 숫자만 포함될 수 있습니다.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As configurações podem conter apenas letras e números</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Настройки могут содержать только буквы и цифры.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mipangilio inaweza kuwa barua na nambari tu.</t>
-  </si>
-  <si>
-    <t>设置只能包含字母和数字</t>
+    <t xml:space="preserve">Password and access keys can only include letters and numbers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">የይለፍ ቃላት እና የመዳረሻ ቁልፎች ፊደላትን እና ቁጥሮችን ብቻ ሊይዙ ይችላሉ።</t>
+  </si>
+  <si>
+    <t xml:space="preserve">يجب أن تحتوي كلمات المرور ومفاتيح الوصول على أحرف وأرقام فقط.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passwörter und Zugangsschlüssel dürfen nur Buchstaben und Zahlen enthalten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رمزهای عبور و کلیدهای دسترسی فقط می‌توانند شامل حروف و اعداد باشند.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las contraseñas y las claves de acceso solo pueden contener letras y números.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les mots de passe et les clés d'accès ne peuvent contenir que des lettres et des chiffres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סיסמאות ומפתחות גישה יכולים להכיל רק אותיות ומספרים.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">पासवर्ड और एक्सेस की में सिर्फ़ अक्षर और नंबर हो सकते हैं।</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le password e le chiavi di accesso possono contenere solo lettere e numeri.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">비밀번호와 접근 키에는 문자 및 숫자만 사용할 수 있습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As palavras-passe e as chaves de acesso só podem conter letras e números.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пароли и ключи доступа могут содержать только буквы и цифры.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manenosiri na funguo za ufikiaji zinaweza kuwa na herufi na nambari pekee.</t>
+  </si>
+  <si>
+    <t>密码和访问密钥只能包含字母和数字。</t>
   </si>
   <si>
     <t>MIRROR:MirrorPatientData</t>
@@ -14896,6 +14896,12 @@
   </si>
   <si>
     <t>客户</t>
+  </si>
+  <si>
+    <t>MIRROR:ServerAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server Address:</t>
   </si>
   <si>
     <t>MIRROR:AccessionKey</t>
@@ -15640,10 +15646,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -26494,10 +26500,10 @@
       </c>
     </row>
     <row r="223" s="1" customFormat="1">
-      <c r="A223" s="6" t="s">
+      <c r="A223" s="1" t="s">
         <v>3021</v>
       </c>
-      <c r="B223" s="6" t="s">
+      <c r="B223" s="1" t="s">
         <v>1116</v>
       </c>
       <c r="C223" s="1" t="s">
@@ -27247,49 +27253,49 @@
       <c r="A238" s="1" t="s">
         <v>3240</v>
       </c>
-      <c r="B238" s="7" t="s">
+      <c r="B238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="C238" s="7" t="s">
+      <c r="C238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="D238" s="7" t="s">
+      <c r="D238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="E238" s="7" t="s">
+      <c r="E238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="F238" s="7" t="s">
+      <c r="F238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="G238" s="7" t="s">
+      <c r="G238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="H238" s="7" t="s">
+      <c r="H238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="I238" s="7" t="s">
+      <c r="I238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="J238" s="7" t="s">
+      <c r="J238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="K238" s="7" t="s">
+      <c r="K238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="L238" s="7" t="s">
+      <c r="L238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="M238" s="7" t="s">
+      <c r="M238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="N238" s="7" t="s">
+      <c r="N238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="O238" s="7" t="s">
+      <c r="O238" s="6" t="s">
         <v>3241</v>
       </c>
-      <c r="P238" s="7" t="s">
+      <c r="P238" s="6" t="s">
         <v>3241</v>
       </c>
     </row>
@@ -27297,49 +27303,49 @@
       <c r="A239" s="1" t="s">
         <v>3242</v>
       </c>
-      <c r="B239" s="7" t="s">
+      <c r="B239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="C239" s="7" t="s">
+      <c r="C239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="D239" s="7" t="s">
+      <c r="D239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="E239" s="7" t="s">
+      <c r="E239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="F239" s="7" t="s">
+      <c r="F239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="G239" s="7" t="s">
+      <c r="G239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="H239" s="7" t="s">
+      <c r="H239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="I239" s="7" t="s">
+      <c r="I239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="J239" s="7" t="s">
+      <c r="J239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="K239" s="7" t="s">
+      <c r="K239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="L239" s="7" t="s">
+      <c r="L239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="M239" s="7" t="s">
+      <c r="M239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="N239" s="7" t="s">
+      <c r="N239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="O239" s="7" t="s">
+      <c r="O239" s="6" t="s">
         <v>3243</v>
       </c>
-      <c r="P239" s="7" t="s">
+      <c r="P239" s="6" t="s">
         <v>3243</v>
       </c>
     </row>
@@ -27347,49 +27353,49 @@
       <c r="A240" s="1" t="s">
         <v>3244</v>
       </c>
-      <c r="B240" s="7" t="s">
+      <c r="B240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="C240" s="7" t="s">
+      <c r="C240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="D240" s="7" t="s">
+      <c r="D240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="E240" s="7" t="s">
+      <c r="E240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="F240" s="7" t="s">
+      <c r="F240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="G240" s="7" t="s">
+      <c r="G240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="H240" s="7" t="s">
+      <c r="H240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="I240" s="7" t="s">
+      <c r="I240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="J240" s="7" t="s">
+      <c r="J240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="K240" s="7" t="s">
+      <c r="K240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="L240" s="7" t="s">
+      <c r="L240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="M240" s="7" t="s">
+      <c r="M240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="N240" s="7" t="s">
+      <c r="N240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="O240" s="7" t="s">
+      <c r="O240" s="6" t="s">
         <v>3245</v>
       </c>
-      <c r="P240" s="7" t="s">
+      <c r="P240" s="6" t="s">
         <v>3245</v>
       </c>
     </row>
@@ -34713,7 +34719,7 @@
       <c r="A400" s="1" t="s">
         <v>4885</v>
       </c>
-      <c r="B400" s="1" t="s">
+      <c r="B400" s="7" t="s">
         <v>4886</v>
       </c>
       <c r="C400" s="1" t="s">
@@ -35017,696 +35023,746 @@
         <v>4961</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>4962</v>
+        <v>4936</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>4963</v>
+        <v>4937</v>
       </c>
       <c r="E406" s="1" t="s">
-        <v>4964</v>
+        <v>4935</v>
       </c>
       <c r="F406" s="1" t="s">
-        <v>4965</v>
+        <v>4938</v>
       </c>
       <c r="G406" s="1" t="s">
-        <v>4966</v>
+        <v>4939</v>
       </c>
       <c r="H406" s="1" t="s">
-        <v>4967</v>
+        <v>4940</v>
       </c>
       <c r="I406" s="1" t="s">
-        <v>4968</v>
+        <v>4941</v>
       </c>
       <c r="J406" s="1" t="s">
-        <v>4969</v>
+        <v>4942</v>
       </c>
       <c r="K406" s="1" t="s">
-        <v>4970</v>
+        <v>4935</v>
       </c>
       <c r="L406" s="1" t="s">
-        <v>4971</v>
+        <v>4943</v>
       </c>
       <c r="M406" s="1" t="s">
-        <v>4972</v>
+        <v>4939</v>
       </c>
       <c r="N406" s="1" t="s">
-        <v>4973</v>
+        <v>4944</v>
       </c>
       <c r="O406" s="1" t="s">
-        <v>4974</v>
+        <v>4945</v>
       </c>
       <c r="P406" s="1" t="s">
-        <v>4975</v>
+        <v>4946</v>
       </c>
     </row>
     <row r="407" s="1" customFormat="1">
       <c r="A407" s="1" t="s">
+        <v>4962</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>4963</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>4964</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>4965</v>
+      </c>
+      <c r="E407" s="1" t="s">
+        <v>4966</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>4967</v>
+      </c>
+      <c r="G407" s="1" t="s">
+        <v>4968</v>
+      </c>
+      <c r="H407" s="1" t="s">
+        <v>4969</v>
+      </c>
+      <c r="I407" s="1" t="s">
+        <v>4970</v>
+      </c>
+      <c r="J407" s="1" t="s">
+        <v>4971</v>
+      </c>
+      <c r="K407" s="1" t="s">
+        <v>4972</v>
+      </c>
+      <c r="L407" s="1" t="s">
+        <v>4973</v>
+      </c>
+      <c r="M407" s="1" t="s">
+        <v>4974</v>
+      </c>
+      <c r="N407" s="1" t="s">
+        <v>4975</v>
+      </c>
+      <c r="O407" s="1" t="s">
         <v>4976</v>
       </c>
-      <c r="B407" s="1" t="s">
+      <c r="P407" s="1" t="s">
         <v>4977</v>
-      </c>
-      <c r="C407" s="1" t="s">
-        <v>4978</v>
-      </c>
-      <c r="D407" s="1" t="s">
-        <v>4979</v>
-      </c>
-      <c r="E407" s="1" t="s">
-        <v>4980</v>
-      </c>
-      <c r="F407" s="1" t="s">
-        <v>4981</v>
-      </c>
-      <c r="G407" s="1" t="s">
-        <v>4982</v>
-      </c>
-      <c r="H407" s="1" t="s">
-        <v>4983</v>
-      </c>
-      <c r="I407" s="1" t="s">
-        <v>4984</v>
-      </c>
-      <c r="J407" s="1" t="s">
-        <v>4985</v>
-      </c>
-      <c r="K407" s="1" t="s">
-        <v>4986</v>
-      </c>
-      <c r="L407" s="1" t="s">
-        <v>4987</v>
-      </c>
-      <c r="M407" s="1" t="s">
-        <v>4988</v>
-      </c>
-      <c r="N407" s="1" t="s">
-        <v>4989</v>
-      </c>
-      <c r="O407" s="1" t="s">
-        <v>4990</v>
-      </c>
-      <c r="P407" s="1" t="s">
-        <v>4991</v>
       </c>
     </row>
     <row r="408" s="1" customFormat="1">
       <c r="A408" s="1" t="s">
+        <v>4978</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>4979</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>4980</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>4981</v>
+      </c>
+      <c r="E408" s="1" t="s">
+        <v>4982</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>4983</v>
+      </c>
+      <c r="G408" s="1" t="s">
+        <v>4984</v>
+      </c>
+      <c r="H408" s="1" t="s">
+        <v>4985</v>
+      </c>
+      <c r="I408" s="1" t="s">
+        <v>4986</v>
+      </c>
+      <c r="J408" s="1" t="s">
+        <v>4987</v>
+      </c>
+      <c r="K408" s="1" t="s">
+        <v>4988</v>
+      </c>
+      <c r="L408" s="1" t="s">
+        <v>4989</v>
+      </c>
+      <c r="M408" s="1" t="s">
+        <v>4990</v>
+      </c>
+      <c r="N408" s="1" t="s">
+        <v>4991</v>
+      </c>
+      <c r="O408" s="1" t="s">
         <v>4992</v>
       </c>
-      <c r="B408" s="1" t="s">
+      <c r="P408" s="1" t="s">
         <v>4993</v>
-      </c>
-      <c r="C408" s="1" t="s">
-        <v>4994</v>
-      </c>
-      <c r="D408" s="1" t="s">
-        <v>4995</v>
-      </c>
-      <c r="E408" s="1" t="s">
-        <v>4996</v>
-      </c>
-      <c r="F408" s="1" t="s">
-        <v>4997</v>
-      </c>
-      <c r="G408" s="1" t="s">
-        <v>4998</v>
-      </c>
-      <c r="H408" s="1" t="s">
-        <v>4999</v>
-      </c>
-      <c r="I408" s="1" t="s">
-        <v>5000</v>
-      </c>
-      <c r="J408" s="1" t="s">
-        <v>5001</v>
-      </c>
-      <c r="K408" s="1" t="s">
-        <v>5002</v>
-      </c>
-      <c r="L408" s="1" t="s">
-        <v>5003</v>
-      </c>
-      <c r="M408" s="1" t="s">
-        <v>5004</v>
-      </c>
-      <c r="N408" s="1" t="s">
-        <v>5005</v>
-      </c>
-      <c r="O408" s="1" t="s">
-        <v>5006</v>
-      </c>
-      <c r="P408" s="1" t="s">
-        <v>5007</v>
       </c>
     </row>
     <row r="409" s="1" customFormat="1">
       <c r="A409" s="1" t="s">
+        <v>4994</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>4995</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>4996</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>4997</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>4998</v>
+      </c>
+      <c r="F409" s="1" t="s">
+        <v>4999</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>5000</v>
+      </c>
+      <c r="H409" s="1" t="s">
+        <v>5001</v>
+      </c>
+      <c r="I409" s="1" t="s">
+        <v>5002</v>
+      </c>
+      <c r="J409" s="1" t="s">
+        <v>5003</v>
+      </c>
+      <c r="K409" s="1" t="s">
+        <v>5004</v>
+      </c>
+      <c r="L409" s="1" t="s">
+        <v>5005</v>
+      </c>
+      <c r="M409" s="1" t="s">
+        <v>5006</v>
+      </c>
+      <c r="N409" s="1" t="s">
+        <v>5007</v>
+      </c>
+      <c r="O409" s="1" t="s">
         <v>5008</v>
       </c>
-      <c r="B409" s="1" t="s">
+      <c r="P409" s="1" t="s">
         <v>5009</v>
-      </c>
-      <c r="C409" s="1" t="s">
-        <v>5010</v>
-      </c>
-      <c r="D409" s="1" t="s">
-        <v>5011</v>
-      </c>
-      <c r="E409" s="1" t="s">
-        <v>5012</v>
-      </c>
-      <c r="F409" s="1" t="s">
-        <v>5013</v>
-      </c>
-      <c r="G409" s="1" t="s">
-        <v>5014</v>
-      </c>
-      <c r="H409" s="1" t="s">
-        <v>5015</v>
-      </c>
-      <c r="I409" s="1" t="s">
-        <v>5016</v>
-      </c>
-      <c r="J409" s="1" t="s">
-        <v>5017</v>
-      </c>
-      <c r="K409" s="1" t="s">
-        <v>5018</v>
-      </c>
-      <c r="L409" s="1" t="s">
-        <v>5019</v>
-      </c>
-      <c r="M409" s="1" t="s">
-        <v>5020</v>
-      </c>
-      <c r="N409" s="1" t="s">
-        <v>5021</v>
-      </c>
-      <c r="O409" s="1" t="s">
-        <v>5022</v>
-      </c>
-      <c r="P409" s="1" t="s">
-        <v>5023</v>
       </c>
     </row>
     <row r="410" s="1" customFormat="1">
       <c r="A410" s="1" t="s">
+        <v>5010</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>5011</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>5012</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>5013</v>
+      </c>
+      <c r="E410" s="1" t="s">
+        <v>5014</v>
+      </c>
+      <c r="F410" s="1" t="s">
+        <v>5015</v>
+      </c>
+      <c r="G410" s="1" t="s">
+        <v>5016</v>
+      </c>
+      <c r="H410" s="1" t="s">
+        <v>5017</v>
+      </c>
+      <c r="I410" s="1" t="s">
+        <v>5018</v>
+      </c>
+      <c r="J410" s="1" t="s">
+        <v>5019</v>
+      </c>
+      <c r="K410" s="1" t="s">
+        <v>5020</v>
+      </c>
+      <c r="L410" s="1" t="s">
+        <v>5021</v>
+      </c>
+      <c r="M410" s="1" t="s">
+        <v>5022</v>
+      </c>
+      <c r="N410" s="1" t="s">
+        <v>5023</v>
+      </c>
+      <c r="O410" s="1" t="s">
         <v>5024</v>
       </c>
-      <c r="B410" s="1" t="s">
+      <c r="P410" s="1" t="s">
         <v>5025</v>
-      </c>
-      <c r="C410" s="1" t="s">
-        <v>5026</v>
-      </c>
-      <c r="D410" s="1" t="s">
-        <v>5027</v>
-      </c>
-      <c r="E410" s="1" t="s">
-        <v>5028</v>
-      </c>
-      <c r="F410" s="1" t="s">
-        <v>5029</v>
-      </c>
-      <c r="G410" s="1" t="s">
-        <v>5030</v>
-      </c>
-      <c r="H410" s="1" t="s">
-        <v>5031</v>
-      </c>
-      <c r="I410" s="1" t="s">
-        <v>5032</v>
-      </c>
-      <c r="J410" s="1" t="s">
-        <v>5033</v>
-      </c>
-      <c r="K410" s="1" t="s">
-        <v>5034</v>
-      </c>
-      <c r="L410" s="1" t="s">
-        <v>5035</v>
-      </c>
-      <c r="M410" s="1" t="s">
-        <v>5036</v>
-      </c>
-      <c r="N410" s="1" t="s">
-        <v>5037</v>
-      </c>
-      <c r="O410" s="1" t="s">
-        <v>5038</v>
-      </c>
-      <c r="P410" s="1" t="s">
-        <v>5039</v>
       </c>
     </row>
     <row r="411" s="1" customFormat="1">
       <c r="A411" s="1" t="s">
+        <v>5026</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>5027</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>5028</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>5029</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>5030</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>5031</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>5032</v>
+      </c>
+      <c r="H411" s="1" t="s">
+        <v>5033</v>
+      </c>
+      <c r="I411" s="1" t="s">
+        <v>5034</v>
+      </c>
+      <c r="J411" s="1" t="s">
+        <v>5035</v>
+      </c>
+      <c r="K411" s="1" t="s">
+        <v>5036</v>
+      </c>
+      <c r="L411" s="1" t="s">
+        <v>5037</v>
+      </c>
+      <c r="M411" s="1" t="s">
+        <v>5038</v>
+      </c>
+      <c r="N411" s="1" t="s">
+        <v>5039</v>
+      </c>
+      <c r="O411" s="1" t="s">
         <v>5040</v>
       </c>
-      <c r="B411" s="1" t="s">
+      <c r="P411" s="1" t="s">
         <v>5041</v>
       </c>
-      <c r="C411" s="1" t="s">
+    </row>
+    <row r="412" s="1" customFormat="1">
+      <c r="A412" s="1" t="s">
         <v>5042</v>
       </c>
-      <c r="D411" s="1" t="s">
+      <c r="B412" s="1" t="s">
         <v>5043</v>
       </c>
-      <c r="E411" s="1" t="s">
+      <c r="C412" s="1" t="s">
         <v>5044</v>
       </c>
-      <c r="F411" s="1" t="s">
+      <c r="D412" s="1" t="s">
         <v>5045</v>
       </c>
-      <c r="G411" s="1" t="s">
+      <c r="E412" s="1" t="s">
         <v>5046</v>
       </c>
-      <c r="H411" s="1" t="s">
+      <c r="F412" s="1" t="s">
         <v>5047</v>
       </c>
-      <c r="I411" s="1" t="s">
+      <c r="G412" s="1" t="s">
         <v>5048</v>
       </c>
-      <c r="J411" s="1" t="s">
+      <c r="H412" s="1" t="s">
         <v>5049</v>
       </c>
-      <c r="K411" s="1" t="s">
+      <c r="I412" s="1" t="s">
         <v>5050</v>
       </c>
-      <c r="L411" s="1" t="s">
+      <c r="J412" s="1" t="s">
         <v>5051</v>
       </c>
-      <c r="M411" s="1" t="s">
+      <c r="K412" s="1" t="s">
         <v>5052</v>
       </c>
-      <c r="N411" s="1" t="s">
+      <c r="L412" s="1" t="s">
         <v>5053</v>
       </c>
-      <c r="O411" s="1" t="s">
+      <c r="M412" s="1" t="s">
         <v>5054</v>
       </c>
-      <c r="P411" s="1" t="s">
+      <c r="N412" s="1" t="s">
         <v>5055</v>
       </c>
-    </row>
-    <row r="413" s="1" customFormat="1">
-      <c r="A413" s="1" t="s">
+      <c r="O412" s="1" t="s">
         <v>5056</v>
       </c>
-      <c r="B413" s="1" t="s">
+      <c r="P412" s="1" t="s">
         <v>5057</v>
-      </c>
-      <c r="C413" s="1" t="s">
-        <v>5058</v>
-      </c>
-      <c r="D413" s="1" t="s">
-        <v>5059</v>
-      </c>
-      <c r="E413" s="1" t="s">
-        <v>3557</v>
-      </c>
-      <c r="F413" s="1" t="s">
-        <v>5060</v>
-      </c>
-      <c r="G413" s="1" t="s">
-        <v>5061</v>
-      </c>
-      <c r="H413" s="1" t="s">
-        <v>5062</v>
-      </c>
-      <c r="I413" s="1" t="s">
-        <v>5063</v>
-      </c>
-      <c r="J413" s="1" t="s">
-        <v>5064</v>
-      </c>
-      <c r="K413" s="1" t="s">
-        <v>5065</v>
-      </c>
-      <c r="L413" s="1" t="s">
-        <v>5066</v>
-      </c>
-      <c r="M413" s="1" t="s">
-        <v>5067</v>
-      </c>
-      <c r="N413" s="1" t="s">
-        <v>5068</v>
-      </c>
-      <c r="O413" s="1" t="s">
-        <v>5069</v>
-      </c>
-      <c r="P413" s="1" t="s">
-        <v>5070</v>
       </c>
     </row>
     <row r="414" s="1" customFormat="1">
       <c r="A414" s="1" t="s">
+        <v>5058</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>5059</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>5060</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>5061</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>3557</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>5062</v>
+      </c>
+      <c r="G414" s="1" t="s">
+        <v>5063</v>
+      </c>
+      <c r="H414" s="1" t="s">
+        <v>5064</v>
+      </c>
+      <c r="I414" s="1" t="s">
+        <v>5065</v>
+      </c>
+      <c r="J414" s="1" t="s">
+        <v>5066</v>
+      </c>
+      <c r="K414" s="1" t="s">
+        <v>5067</v>
+      </c>
+      <c r="L414" s="1" t="s">
+        <v>5068</v>
+      </c>
+      <c r="M414" s="1" t="s">
+        <v>5069</v>
+      </c>
+      <c r="N414" s="1" t="s">
+        <v>5070</v>
+      </c>
+      <c r="O414" s="1" t="s">
         <v>5071</v>
       </c>
-      <c r="B414" s="1" t="s">
+      <c r="P414" s="1" t="s">
         <v>5072</v>
-      </c>
-      <c r="C414" s="1" t="s">
-        <v>5073</v>
-      </c>
-      <c r="D414" s="1" t="s">
-        <v>5074</v>
-      </c>
-      <c r="E414" s="1" t="s">
-        <v>5075</v>
-      </c>
-      <c r="F414" s="1" t="s">
-        <v>5076</v>
-      </c>
-      <c r="G414" s="1" t="s">
-        <v>5077</v>
-      </c>
-      <c r="H414" s="1" t="s">
-        <v>5078</v>
-      </c>
-      <c r="I414" s="1" t="s">
-        <v>5079</v>
-      </c>
-      <c r="J414" s="1" t="s">
-        <v>5080</v>
-      </c>
-      <c r="K414" s="1" t="s">
-        <v>5081</v>
-      </c>
-      <c r="L414" s="1" t="s">
-        <v>5082</v>
-      </c>
-      <c r="M414" s="1" t="s">
-        <v>5083</v>
-      </c>
-      <c r="N414" s="1" t="s">
-        <v>5084</v>
-      </c>
-      <c r="O414" s="1" t="s">
-        <v>5085</v>
-      </c>
-      <c r="P414" s="1" t="s">
-        <v>5086</v>
       </c>
     </row>
     <row r="415" s="1" customFormat="1">
       <c r="A415" s="1" t="s">
+        <v>5073</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>5074</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>5075</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>5076</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>5077</v>
+      </c>
+      <c r="F415" s="1" t="s">
+        <v>5078</v>
+      </c>
+      <c r="G415" s="1" t="s">
+        <v>5079</v>
+      </c>
+      <c r="H415" s="1" t="s">
+        <v>5080</v>
+      </c>
+      <c r="I415" s="1" t="s">
+        <v>5081</v>
+      </c>
+      <c r="J415" s="1" t="s">
+        <v>5082</v>
+      </c>
+      <c r="K415" s="1" t="s">
+        <v>5083</v>
+      </c>
+      <c r="L415" s="1" t="s">
+        <v>5084</v>
+      </c>
+      <c r="M415" s="1" t="s">
+        <v>5085</v>
+      </c>
+      <c r="N415" s="1" t="s">
+        <v>5086</v>
+      </c>
+      <c r="O415" s="1" t="s">
         <v>5087</v>
       </c>
-      <c r="B415" s="1" t="s">
+      <c r="P415" s="1" t="s">
         <v>5088</v>
-      </c>
-      <c r="C415" s="1" t="s">
-        <v>5089</v>
-      </c>
-      <c r="D415" s="1" t="s">
-        <v>5090</v>
-      </c>
-      <c r="E415" s="1" t="s">
-        <v>5091</v>
-      </c>
-      <c r="F415" s="1" t="s">
-        <v>5092</v>
-      </c>
-      <c r="G415" s="1" t="s">
-        <v>5093</v>
-      </c>
-      <c r="H415" s="1" t="s">
-        <v>5094</v>
-      </c>
-      <c r="I415" s="1" t="s">
-        <v>5095</v>
-      </c>
-      <c r="J415" s="1" t="s">
-        <v>5096</v>
-      </c>
-      <c r="K415" s="1" t="s">
-        <v>5097</v>
-      </c>
-      <c r="L415" s="1" t="s">
-        <v>5098</v>
-      </c>
-      <c r="M415" s="1" t="s">
-        <v>5099</v>
-      </c>
-      <c r="N415" s="1" t="s">
-        <v>5100</v>
-      </c>
-      <c r="O415" s="1" t="s">
-        <v>5101</v>
-      </c>
-      <c r="P415" s="1" t="s">
-        <v>5102</v>
       </c>
     </row>
     <row r="416" s="1" customFormat="1">
       <c r="A416" s="1" t="s">
+        <v>5089</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>5090</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>5091</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>5092</v>
+      </c>
+      <c r="E416" s="1" t="s">
+        <v>5093</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>5094</v>
+      </c>
+      <c r="G416" s="1" t="s">
+        <v>5095</v>
+      </c>
+      <c r="H416" s="1" t="s">
+        <v>5096</v>
+      </c>
+      <c r="I416" s="1" t="s">
+        <v>5097</v>
+      </c>
+      <c r="J416" s="1" t="s">
+        <v>5098</v>
+      </c>
+      <c r="K416" s="1" t="s">
+        <v>5099</v>
+      </c>
+      <c r="L416" s="1" t="s">
+        <v>5100</v>
+      </c>
+      <c r="M416" s="1" t="s">
+        <v>5101</v>
+      </c>
+      <c r="N416" s="1" t="s">
+        <v>5102</v>
+      </c>
+      <c r="O416" s="1" t="s">
         <v>5103</v>
       </c>
-      <c r="B416" s="1" t="s">
+      <c r="P416" s="1" t="s">
         <v>5104</v>
-      </c>
-      <c r="C416" s="1" t="s">
-        <v>5105</v>
-      </c>
-      <c r="D416" s="1" t="s">
-        <v>5106</v>
-      </c>
-      <c r="E416" s="1" t="s">
-        <v>5107</v>
-      </c>
-      <c r="F416" s="1" t="s">
-        <v>5108</v>
-      </c>
-      <c r="G416" s="1" t="s">
-        <v>5109</v>
-      </c>
-      <c r="H416" s="1" t="s">
-        <v>5110</v>
-      </c>
-      <c r="I416" s="1" t="s">
-        <v>5111</v>
-      </c>
-      <c r="J416" s="1" t="s">
-        <v>5112</v>
-      </c>
-      <c r="K416" s="1" t="s">
-        <v>5113</v>
-      </c>
-      <c r="L416" s="1" t="s">
-        <v>5114</v>
-      </c>
-      <c r="M416" s="1" t="s">
-        <v>5115</v>
-      </c>
-      <c r="N416" s="1" t="s">
-        <v>5116</v>
-      </c>
-      <c r="O416" s="1" t="s">
-        <v>5117</v>
-      </c>
-      <c r="P416" s="1" t="s">
-        <v>5118</v>
       </c>
     </row>
     <row r="417" s="1" customFormat="1">
       <c r="A417" s="1" t="s">
+        <v>5105</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>5106</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>5107</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>5108</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>5109</v>
+      </c>
+      <c r="F417" s="1" t="s">
+        <v>5110</v>
+      </c>
+      <c r="G417" s="1" t="s">
+        <v>5111</v>
+      </c>
+      <c r="H417" s="1" t="s">
+        <v>5112</v>
+      </c>
+      <c r="I417" s="1" t="s">
+        <v>5113</v>
+      </c>
+      <c r="J417" s="1" t="s">
+        <v>5114</v>
+      </c>
+      <c r="K417" s="1" t="s">
+        <v>5115</v>
+      </c>
+      <c r="L417" s="1" t="s">
+        <v>5116</v>
+      </c>
+      <c r="M417" s="1" t="s">
+        <v>5117</v>
+      </c>
+      <c r="N417" s="1" t="s">
+        <v>5118</v>
+      </c>
+      <c r="O417" s="1" t="s">
         <v>5119</v>
       </c>
-      <c r="B417" s="1" t="s">
+      <c r="P417" s="1" t="s">
         <v>5120</v>
-      </c>
-      <c r="C417" s="1" t="s">
-        <v>5121</v>
-      </c>
-      <c r="D417" s="1" t="s">
-        <v>5122</v>
-      </c>
-      <c r="E417" s="1" t="s">
-        <v>5123</v>
-      </c>
-      <c r="F417" s="1" t="s">
-        <v>5124</v>
-      </c>
-      <c r="G417" s="1" t="s">
-        <v>5125</v>
-      </c>
-      <c r="H417" s="1" t="s">
-        <v>5126</v>
-      </c>
-      <c r="I417" s="1" t="s">
-        <v>5127</v>
-      </c>
-      <c r="J417" s="1" t="s">
-        <v>5128</v>
-      </c>
-      <c r="K417" s="1" t="s">
-        <v>5129</v>
-      </c>
-      <c r="L417" s="1" t="s">
-        <v>5130</v>
-      </c>
-      <c r="M417" s="1" t="s">
-        <v>5131</v>
-      </c>
-      <c r="N417" s="1" t="s">
-        <v>5132</v>
-      </c>
-      <c r="O417" s="1" t="s">
-        <v>5133</v>
-      </c>
-      <c r="P417" s="1" t="s">
-        <v>5134</v>
       </c>
     </row>
     <row r="418" s="1" customFormat="1">
       <c r="A418" s="1" t="s">
+        <v>5121</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>5122</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>5123</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>5124</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>5125</v>
+      </c>
+      <c r="F418" s="1" t="s">
+        <v>5126</v>
+      </c>
+      <c r="G418" s="1" t="s">
+        <v>5127</v>
+      </c>
+      <c r="H418" s="1" t="s">
+        <v>5128</v>
+      </c>
+      <c r="I418" s="1" t="s">
+        <v>5129</v>
+      </c>
+      <c r="J418" s="1" t="s">
+        <v>5130</v>
+      </c>
+      <c r="K418" s="1" t="s">
+        <v>5131</v>
+      </c>
+      <c r="L418" s="1" t="s">
+        <v>5132</v>
+      </c>
+      <c r="M418" s="1" t="s">
+        <v>5133</v>
+      </c>
+      <c r="N418" s="1" t="s">
+        <v>5134</v>
+      </c>
+      <c r="O418" s="1" t="s">
         <v>5135</v>
       </c>
-      <c r="B418" s="1" t="s">
+      <c r="P418" s="1" t="s">
         <v>5136</v>
-      </c>
-      <c r="C418" s="1" t="s">
-        <v>5137</v>
-      </c>
-      <c r="D418" s="1" t="s">
-        <v>5138</v>
-      </c>
-      <c r="E418" s="1" t="s">
-        <v>5139</v>
-      </c>
-      <c r="F418" s="1" t="s">
-        <v>5140</v>
-      </c>
-      <c r="G418" s="1" t="s">
-        <v>5141</v>
-      </c>
-      <c r="H418" s="1" t="s">
-        <v>5142</v>
-      </c>
-      <c r="I418" s="1" t="s">
-        <v>5143</v>
-      </c>
-      <c r="J418" s="1" t="s">
-        <v>5144</v>
-      </c>
-      <c r="K418" s="1" t="s">
-        <v>5145</v>
-      </c>
-      <c r="L418" s="1" t="s">
-        <v>5146</v>
-      </c>
-      <c r="M418" s="1" t="s">
-        <v>5147</v>
-      </c>
-      <c r="N418" s="1" t="s">
-        <v>5148</v>
-      </c>
-      <c r="O418" s="1" t="s">
-        <v>5149</v>
-      </c>
-      <c r="P418" s="1" t="s">
-        <v>5150</v>
       </c>
     </row>
     <row r="419" s="1" customFormat="1">
       <c r="A419" s="1" t="s">
+        <v>5137</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>5138</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>5139</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>5140</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>5141</v>
+      </c>
+      <c r="F419" s="1" t="s">
+        <v>5142</v>
+      </c>
+      <c r="G419" s="1" t="s">
+        <v>5143</v>
+      </c>
+      <c r="H419" s="1" t="s">
+        <v>5144</v>
+      </c>
+      <c r="I419" s="1" t="s">
+        <v>5145</v>
+      </c>
+      <c r="J419" s="1" t="s">
+        <v>5146</v>
+      </c>
+      <c r="K419" s="1" t="s">
+        <v>5147</v>
+      </c>
+      <c r="L419" s="1" t="s">
+        <v>5148</v>
+      </c>
+      <c r="M419" s="1" t="s">
+        <v>5149</v>
+      </c>
+      <c r="N419" s="1" t="s">
+        <v>5150</v>
+      </c>
+      <c r="O419" s="1" t="s">
         <v>5151</v>
       </c>
-      <c r="B419" s="1" t="s">
+      <c r="P419" s="1" t="s">
         <v>5152</v>
       </c>
-      <c r="C419" s="1" t="s">
+    </row>
+    <row r="420" s="1" customFormat="1">
+      <c r="A420" s="1" t="s">
         <v>5153</v>
       </c>
-      <c r="D419" s="1" t="s">
+      <c r="B420" s="1" t="s">
         <v>5154</v>
       </c>
-      <c r="E419" s="1" t="s">
+      <c r="C420" s="1" t="s">
         <v>5155</v>
       </c>
-      <c r="F419" s="1" t="s">
+      <c r="D420" s="1" t="s">
         <v>5156</v>
       </c>
-      <c r="G419" s="1" t="s">
+      <c r="E420" s="1" t="s">
         <v>5157</v>
       </c>
-      <c r="H419" s="1" t="s">
+      <c r="F420" s="1" t="s">
         <v>5158</v>
       </c>
-      <c r="I419" s="1" t="s">
+      <c r="G420" s="1" t="s">
         <v>5159</v>
       </c>
-      <c r="J419" s="1" t="s">
+      <c r="H420" s="1" t="s">
         <v>5160</v>
       </c>
-      <c r="K419" s="1" t="s">
+      <c r="I420" s="1" t="s">
         <v>5161</v>
       </c>
-      <c r="L419" s="1" t="s">
+      <c r="J420" s="1" t="s">
         <v>5162</v>
       </c>
-      <c r="M419" s="1" t="s">
+      <c r="K420" s="1" t="s">
         <v>5163</v>
       </c>
-      <c r="N419" s="1" t="s">
+      <c r="L420" s="1" t="s">
         <v>5164</v>
       </c>
-      <c r="O419" s="1" t="s">
+      <c r="M420" s="1" t="s">
         <v>5165</v>
       </c>
-      <c r="P419" s="1" t="s">
+      <c r="N420" s="1" t="s">
         <v>5166</v>
       </c>
-    </row>
-    <row r="420" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A420" s="1" t="s">
+      <c r="O420" s="1" t="s">
         <v>5167</v>
       </c>
-      <c r="B420" s="1" t="s">
+      <c r="P420" s="1" t="s">
         <v>5168</v>
       </c>
-      <c r="C420" s="1" t="s">
+    </row>
+    <row r="421" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A421" s="1" t="s">
         <v>5169</v>
       </c>
-      <c r="D420" s="1" t="s">
+      <c r="B421" s="1" t="s">
         <v>5170</v>
       </c>
-      <c r="E420" s="1" t="s">
+      <c r="C421" s="1" t="s">
         <v>5171</v>
       </c>
-      <c r="F420" s="1" t="s">
+      <c r="D421" s="1" t="s">
         <v>5172</v>
       </c>
-      <c r="G420" s="1" t="s">
+      <c r="E421" s="1" t="s">
         <v>5173</v>
       </c>
-      <c r="H420" s="1" t="s">
+      <c r="F421" s="1" t="s">
         <v>5174</v>
       </c>
-      <c r="I420" s="1" t="s">
+      <c r="G421" s="1" t="s">
         <v>5175</v>
       </c>
-      <c r="J420" s="1" t="s">
+      <c r="H421" s="1" t="s">
         <v>5176</v>
       </c>
-      <c r="K420" s="1" t="s">
+      <c r="I421" s="1" t="s">
         <v>5177</v>
       </c>
-      <c r="L420" s="1" t="s">
+      <c r="J421" s="1" t="s">
         <v>5178</v>
       </c>
-      <c r="M420" s="3" t="s">
+      <c r="K421" s="1" t="s">
         <v>5179</v>
       </c>
-      <c r="N420" s="1" t="s">
+      <c r="L421" s="1" t="s">
         <v>5180</v>
       </c>
-      <c r="O420" s="1" t="s">
+      <c r="M421" s="3" t="s">
         <v>5181</v>
       </c>
-      <c r="P420" s="1" t="s">
+      <c r="N421" s="1" t="s">
         <v>5182</v>
+      </c>
+      <c r="O421" s="1" t="s">
+        <v>5183</v>
+      </c>
+      <c r="P421" s="1" t="s">
+        <v>5184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>